<commit_message>
Dokumentation fertig gestellt - Abgabe Phase 2
</commit_message>
<xml_diff>
--- a/dok/1.1 Konzeptionsphase/Einzelnen Dokumente Phase 1/Zeitplan GANNT.xlsx
+++ b/dok/1.1 Konzeptionsphase/Einzelnen Dokumente Phase 1/Zeitplan GANNT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\OneDrive\Desktop\Projekt\repo\dok\1.1 Konzeptionsphase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\OneDrive\Desktop\Projekt\repo\dok\1.1 Konzeptionsphase\Einzelnen Dokumente Phase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2388D3EE-54BE-4C14-8D38-C45907552EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EC76BC-8813-4FA4-B4AF-212174CB0FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36B9B559-1347-1E4F-AF8F-ABE1F2AFADA3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Start</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Kevin Walter</t>
+  </si>
+  <si>
+    <t>Erarbeitungsphase abgeschlossen</t>
+  </si>
+  <si>
+    <t>M6</t>
   </si>
 </sst>
 </file>
@@ -245,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -282,9 +288,6 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -295,12 +298,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -309,34 +314,9 @@
       </fill>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFFF0000"/>
-        </left>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -497,23 +477,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Raute 7">
+        <xdr:cNvPr id="9" name="Raute 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E2D8B2C-CE98-4EF6-A924-CFBBF58591BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC3B1C03-6AE8-4632-92EC-57F653F2EA7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -521,7 +501,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10277475" y="4572000"/>
+          <a:off x="11449050" y="5981700"/>
           <a:ext cx="180975" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -560,23 +540,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Raute 8">
+        <xdr:cNvPr id="10" name="Raute 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC3B1C03-6AE8-4632-92EC-57F653F2EA7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6B0FF93-A227-4C79-9ED2-2E7255C4539D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -584,7 +564,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11163300" y="5781675"/>
+          <a:off x="12058650" y="6581775"/>
           <a:ext cx="180975" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -623,23 +603,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Raute 9">
+        <xdr:cNvPr id="2" name="Raute 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6B0FF93-A227-4C79-9ED2-2E7255C4539D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{688C32AB-CB85-4E9E-A3B5-D4E727CDEC03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -647,7 +627,70 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11753850" y="6381750"/>
+          <a:off x="10277475" y="4581525"/>
+          <a:ext cx="180975" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Raute 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B5DCE0F-7E00-46D1-98D7-DF08A7641CA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10572750" y="5181600"/>
           <a:ext cx="180975" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -987,10 +1030,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AN59"/>
+  <dimension ref="A1:AL61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN13" sqref="AN13"/>
+      <selection activeCell="AA34" sqref="AA34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1005,14 +1048,14 @@
     <col min="30" max="37" width="3.875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="11.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:40" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="1" spans="1:38" ht="11.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:38" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14"/>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B2" s="18"/>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1063,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1028,7 +1071,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1036,9 +1079,9 @@
         <v>45836</v>
       </c>
     </row>
-    <row r="7" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:40" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+    <row r="7" spans="1:38" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:38" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1177,13 +1220,12 @@
         <f t="shared" si="0"/>
         <v>45866</v>
       </c>
-      <c r="AN8" s="19"/>
-    </row>
-    <row r="9" spans="1:40" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:38" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="5" t="s">
         <v>7</v>
@@ -1224,8 +1266,8 @@
       <c r="AK10" s="3"/>
       <c r="AL10" s="3"/>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
         <v>1.1000000000000001</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1274,8 +1316,8 @@
       <c r="AK11" s="7"/>
       <c r="AL11" s="3"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
         <v>1.2</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1288,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="11">
-        <f t="shared" ref="C12:E29" si="1">IF(C12&gt;=0.01,C12+D12,"")</f>
+        <f t="shared" ref="E12:E31" si="1">IF(C12&gt;=0.01,C12+D12,"")</f>
         <v>45838</v>
       </c>
       <c r="G12" s="7"/>
@@ -1324,8 +1366,8 @@
       <c r="AK12" s="7"/>
       <c r="AL12" s="3"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
         <v>1.3</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1374,8 +1416,8 @@
       <c r="AK13" s="7"/>
       <c r="AL13" s="3"/>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
         <v>1.4</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1424,8 +1466,8 @@
       <c r="AK14" s="7"/>
       <c r="AL14" s="3"/>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1442,7 +1484,7 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="18"/>
+      <c r="K15" s="17"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
@@ -1471,8 +1513,8 @@
       <c r="AK15" s="7"/>
       <c r="AL15" s="3"/>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
       <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
@@ -1516,7 +1558,7 @@
       <c r="AL16" s="3"/>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <v>2.1</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1566,7 +1608,7 @@
       <c r="AL17" s="3"/>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
+      <c r="A18" s="15">
         <v>2.2000000000000002</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1616,7 +1658,7 @@
       <c r="AL18" s="3"/>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1641,7 +1683,7 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
-      <c r="S19" s="18"/>
+      <c r="S19" s="17"/>
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
       <c r="V19" s="7"/>
@@ -1663,11 +1705,11 @@
       <c r="AL19" s="3"/>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
+      <c r="A20" s="15">
         <v>2.2999999999999998</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C20" s="10">
         <v>45848</v>
@@ -1713,17 +1755,17 @@
       <c r="AL20" s="3"/>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C21" s="10">
         <v>45850</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="10">
+      <c r="E21" s="11">
         <v>45850</v>
       </c>
       <c r="G21" s="7"/>
@@ -1740,7 +1782,7 @@
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
-      <c r="U21" s="18"/>
+      <c r="U21" s="17"/>
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
@@ -1760,20 +1802,15 @@
       <c r="AL21" s="3"/>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
-        <v>2.4</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="10">
-        <v>45836</v>
-      </c>
-      <c r="D22" s="6">
-        <v>12</v>
-      </c>
-      <c r="E22" s="10">
-        <v>45850</v>
+      <c r="A22" s="15"/>
+      <c r="B22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -1809,15 +1846,20 @@
       <c r="AL22" s="3"/>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A23" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="10">
+        <v>45850</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2</v>
+      </c>
+      <c r="E23" s="11">
+        <v>45851</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -1853,20 +1895,17 @@
       <c r="AL23" s="3"/>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
-        <v>3.1</v>
+      <c r="A24" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C24" s="10">
-        <v>45850</v>
-      </c>
-      <c r="D24" s="6">
-        <v>1</v>
-      </c>
-      <c r="E24" s="11">
-        <f t="shared" si="1"/>
+        <v>45851</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="10">
         <v>45851</v>
       </c>
       <c r="G24" s="7"/>
@@ -1884,7 +1923,7 @@
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
+      <c r="V24" s="17"/>
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
       <c r="Y24" s="7"/>
@@ -1903,13 +1942,13 @@
       <c r="AL24" s="3"/>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A25" s="16">
+      <c r="A25" s="15">
         <v>3.2</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="11">
+        <v>18</v>
+      </c>
+      <c r="C25" s="10">
         <v>45851</v>
       </c>
       <c r="D25" s="6">
@@ -1953,13 +1992,13 @@
       <c r="AL25" s="3"/>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
+      <c r="A26" s="15">
         <v>3.3</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="10">
+        <v>19</v>
+      </c>
+      <c r="C26" s="11">
         <v>45852</v>
       </c>
       <c r="D26" s="6">
@@ -2003,18 +2042,21 @@
       <c r="AL26" s="3"/>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>30</v>
+      <c r="A27" s="15">
+        <v>3.4</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C27" s="10">
         <v>45853</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="10">
-        <v>45853</v>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="11">
+        <f t="shared" si="1"/>
+        <v>45854</v>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
@@ -2033,7 +2075,7 @@
       <c r="U27" s="7"/>
       <c r="V27" s="7"/>
       <c r="W27" s="7"/>
-      <c r="X27" s="18"/>
+      <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
       <c r="AA27" s="7"/>
@@ -2050,20 +2092,17 @@
       <c r="AL27" s="3"/>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A28" s="16">
-        <v>3.4</v>
+      <c r="A28" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C28" s="10">
-        <v>45853</v>
-      </c>
-      <c r="D28" s="6">
-        <v>1</v>
-      </c>
-      <c r="E28" s="11">
-        <f t="shared" si="1"/>
+        <v>45854</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="10">
         <v>45854</v>
       </c>
       <c r="G28" s="7"/>
@@ -2084,7 +2123,7 @@
       <c r="V28" s="7"/>
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
-      <c r="Y28" s="7"/>
+      <c r="Y28" s="17"/>
       <c r="Z28" s="7"/>
       <c r="AA28" s="7"/>
       <c r="AB28" s="7"/>
@@ -2100,11 +2139,11 @@
       <c r="AL28" s="3"/>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A29" s="16">
+      <c r="A29" s="15">
         <v>3.5</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C29" s="10">
         <v>45854</v>
@@ -2150,41 +2189,118 @@
       <c r="AL29" s="3"/>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>32</v>
+      <c r="A30" s="15">
+        <v>3.6</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C30" s="10">
         <v>45855</v>
       </c>
-      <c r="D30" s="6"/>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
       <c r="E30" s="11">
-        <v>45855</v>
-      </c>
-      <c r="Z30" s="18"/>
+        <f>IF(C30&gt;=0.01,C30+D30,"")</f>
+        <v>45856</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
+      <c r="AB30" s="7"/>
+      <c r="AC30" s="7"/>
+      <c r="AD30" s="7"/>
+      <c r="AE30" s="7"/>
+      <c r="AF30" s="7"/>
+      <c r="AG30" s="7"/>
+      <c r="AH30" s="7"/>
+      <c r="AI30" s="7"/>
+      <c r="AJ30" s="7"/>
+      <c r="AK30" s="7"/>
+      <c r="AL30" s="3"/>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="10">
+        <v>45856</v>
+      </c>
+      <c r="E31" s="10">
+        <v>45856</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="AA31" s="17"/>
+      <c r="AB31" s="7"/>
+      <c r="AC31" s="7"/>
+      <c r="AD31" s="7"/>
+      <c r="AE31" s="7"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="7"/>
+      <c r="AH31" s="7"/>
+      <c r="AI31" s="7"/>
+      <c r="AJ31" s="7"/>
+      <c r="AK31" s="7"/>
+      <c r="AL31" s="3"/>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
       <c r="D32" s="6"/>
+      <c r="Z32" s="7"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
+      <c r="A33" s="16"/>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
+      <c r="A34" s="16"/>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
       <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="16"/>
       <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2255,21 +2371,43 @@
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <conditionalFormatting sqref="G8:AK8">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>WEEKDAY(G$8)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:AK14 G16:AK18 G15:J15 L15:AK15 G20:AK20 G19:R19 T19:AK19 G22:AK26 G21:T21 V21:AK21 G28:AK29 G27:W27 Y27:AK27">
-    <cfRule type="expression" dxfId="5" priority="10">
+  <conditionalFormatting sqref="G11:AK14 G15:J15 L15:AK15 G16:AK18 G19:R19 T19:AK19 G20:AK20 Z28:AK28 G22:AK23 G21:T21 V21:AK21 G25:AK27 G24:U24 W24:AK24 G28:X28 G29:AK29 Z30:AA30">
+    <cfRule type="expression" dxfId="2" priority="12">
       <formula>AND(NOT(ISBLANK($C11)),G$8&gt;=$C11,G$8&lt;=$E11)</formula>
     </cfRule>
-    <cfRule type="expression" priority="11">
+    <cfRule type="expression" priority="13">
+      <formula>ISBLANK(C$11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31:Y31 Z32 AB31:AK31">
+    <cfRule type="expression" dxfId="1" priority="22">
+      <formula>AND(NOT(ISBLANK($C30)),G$8&gt;=$C30,G$8&lt;=$E30)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="23">
+      <formula>ISBLANK(C$11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30:AK30">
+    <cfRule type="expression" dxfId="0" priority="24">
+      <formula>AND(NOT(ISBLANK(#REF!)),G$8&gt;=#REF!,G$8&lt;=#REF!)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="25">
       <formula>ISBLANK(C$11)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Anpassungen im Dokument nach Feedback
</commit_message>
<xml_diff>
--- a/dok/1.1 Konzeptionsphase/Einzelnen Dokumente Phase 1/Zeitplan GANNT.xlsx
+++ b/dok/1.1 Konzeptionsphase/Einzelnen Dokumente Phase 1/Zeitplan GANNT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\OneDrive\Desktop\Projekt\repo\dok\1.1 Konzeptionsphase\Einzelnen Dokumente Phase 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Projekt\repo\dok\1.1 Konzeptionsphase\Einzelnen Dokumente Phase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EC76BC-8813-4FA4-B4AF-212174CB0FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5695FA6A-32ED-447C-AF4F-E1FE6C471C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36B9B559-1347-1E4F-AF8F-ABE1F2AFADA3}"/>
+    <workbookView xWindow="-19290" yWindow="-3200" windowWidth="19380" windowHeight="11460" xr2:uid="{36B9B559-1347-1E4F-AF8F-ABE1F2AFADA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplan" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Start</t>
   </si>
@@ -75,15 +75,9 @@
     <t>Phase 2: Erarbeitungsphase/Reflexionsphase</t>
   </si>
   <si>
-    <t>Architekturdokument</t>
-  </si>
-  <si>
     <t>Implementierung</t>
   </si>
   <si>
-    <t>Unit-Tests</t>
-  </si>
-  <si>
     <t>GitHub-Integration</t>
   </si>
   <si>
@@ -129,21 +123,9 @@
     <t>M4</t>
   </si>
   <si>
-    <t>Dokumentation abgeschlossen</t>
-  </si>
-  <si>
-    <t>M5</t>
-  </si>
-  <si>
     <t>Projekt abgeschlossen / Finale abgabe</t>
   </si>
   <si>
-    <t>Finale Abgabe / alles noch einmal prüfen</t>
-  </si>
-  <si>
-    <t>Projekt SE</t>
-  </si>
-  <si>
     <t>Kevin Walter</t>
   </si>
   <si>
@@ -151,6 +133,66 @@
   </si>
   <si>
     <t>M6</t>
+  </si>
+  <si>
+    <t>Aufgabenplaner</t>
+  </si>
+  <si>
+    <t>Architekturdokument erstellen</t>
+  </si>
+  <si>
+    <t>Persistenzschicht</t>
+  </si>
+  <si>
+    <t>1,3,1</t>
+  </si>
+  <si>
+    <t>UML-Diagramme erstellen</t>
+  </si>
+  <si>
+    <t>2,1,1</t>
+  </si>
+  <si>
+    <t>MVC-Modell und Entkopplung durch Interface</t>
+  </si>
+  <si>
+    <t>2,2,1</t>
+  </si>
+  <si>
+    <t>GUI-Implementierung mit Qt</t>
+  </si>
+  <si>
+    <t>2,2,2</t>
+  </si>
+  <si>
+    <t>Logik (TaskManager)</t>
+  </si>
+  <si>
+    <t>2,2,3</t>
+  </si>
+  <si>
+    <t>Testing (System- und Integrations, Unit-Tests)</t>
+  </si>
+  <si>
+    <t>GoogleTest für automatisierte Unit-Tests</t>
+  </si>
+  <si>
+    <t>3,1,1</t>
+  </si>
+  <si>
+    <t>Dokumentation der Testergebnisse</t>
+  </si>
+  <si>
+    <t>3,2,1</t>
+  </si>
+  <si>
+    <t>3,3,1</t>
+  </si>
+  <si>
+    <t>Beschreibung von Installation/GUI-Elemente</t>
+  </si>
+  <si>
+    <t>Finale Abgabe</t>
   </si>
 </sst>
 </file>
@@ -192,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +262,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -301,11 +349,66 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -334,6 +437,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -351,15 +461,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -375,133 +485,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7172325" y="3381375"/>
-          <a:ext cx="180975" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx1"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="de-DE" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Raute 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09E56F79-4954-4607-9B79-CA0A08822CDD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9677400" y="4181475"/>
-          <a:ext cx="180975" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx1"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="de-DE" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Raute 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC3B1C03-6AE8-4632-92EC-57F653F2EA7C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11449050" y="5981700"/>
+          <a:off x="7629525" y="3581400"/>
           <a:ext cx="180975" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -541,22 +525,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Raute 9">
+        <xdr:cNvPr id="7" name="Raute 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6B0FF93-A227-4C79-9ED2-2E7255C4539D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09E56F79-4954-4607-9B79-CA0A08822CDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -564,7 +548,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12058650" y="6581775"/>
+          <a:off x="12068175" y="5181600"/>
           <a:ext cx="180975" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -603,23 +587,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Raute 1">
+        <xdr:cNvPr id="10" name="Raute 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{688C32AB-CB85-4E9E-A3B5-D4E727CDEC03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6B0FF93-A227-4C79-9ED2-2E7255C4539D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -627,7 +611,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10277475" y="4581525"/>
+          <a:off x="15220950" y="7981950"/>
           <a:ext cx="180975" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -666,16 +650,79 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Raute 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{688C32AB-CB85-4E9E-A3B5-D4E727CDEC03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12353925" y="5581650"/>
+          <a:ext cx="180975" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -690,7 +737,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10572750" y="5181600"/>
+          <a:off x="13411200" y="6372225"/>
           <a:ext cx="180975" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -1030,48 +1077,48 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AL61"/>
+  <dimension ref="A1:AM68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA34" sqref="AA34"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.875" customWidth="1"/>
     <col min="2" max="2" width="38.5" customWidth="1"/>
-    <col min="3" max="3" width="12.25" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.375" customWidth="1"/>
-    <col min="6" max="6" width="0.875" customWidth="1"/>
-    <col min="7" max="29" width="3.875" customWidth="1"/>
-    <col min="30" max="37" width="3.875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="0.875" hidden="1" customWidth="1"/>
+    <col min="7" max="28" width="3.875" customWidth="1"/>
+    <col min="29" max="39" width="3.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="11.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:38" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="11.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:39" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="18"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1079,13 +1126,13 @@
         <v>45836</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:38" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:39" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>0</v>
@@ -1220,12 +1267,18 @@
         <f t="shared" si="0"/>
         <v>45866</v>
       </c>
-    </row>
-    <row r="9" spans="1:38" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL8" s="13">
+        <v>45867</v>
+      </c>
+      <c r="AM8" s="13">
+        <v>45868</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="5" t="s">
         <v>7</v>
@@ -1266,7 +1319,7 @@
       <c r="AK10" s="3"/>
       <c r="AL10" s="3"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>1.1000000000000001</v>
       </c>
@@ -1314,9 +1367,10 @@
       <c r="AI11" s="7"/>
       <c r="AJ11" s="7"/>
       <c r="AK11" s="7"/>
-      <c r="AL11" s="3"/>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL11" s="7"/>
+      <c r="AM11" s="7"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>1.2</v>
       </c>
@@ -1330,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="11">
-        <f t="shared" ref="E12:E31" si="1">IF(C12&gt;=0.01,C12+D12,"")</f>
+        <f t="shared" ref="E12:E35" si="1">IF(C12&gt;=0.01,C12+D12,"")</f>
         <v>45838</v>
       </c>
       <c r="G12" s="7"/>
@@ -1364,9 +1418,10 @@
       <c r="AI12" s="7"/>
       <c r="AJ12" s="7"/>
       <c r="AK12" s="7"/>
-      <c r="AL12" s="3"/>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL12" s="7"/>
+      <c r="AM12" s="7"/>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>1.3</v>
       </c>
@@ -1414,14 +1469,15 @@
       <c r="AI13" s="7"/>
       <c r="AJ13" s="7"/>
       <c r="AK13" s="7"/>
-      <c r="AL13" s="3"/>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
-        <v>1.4</v>
+      <c r="AL13" s="7"/>
+      <c r="AM13" s="7"/>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C14" s="10">
         <v>45839</v>
@@ -1430,7 +1486,6 @@
         <v>1</v>
       </c>
       <c r="E14" s="11">
-        <f t="shared" si="1"/>
         <v>45840</v>
       </c>
       <c r="G14" s="7"/>
@@ -1464,27 +1519,31 @@
       <c r="AI14" s="7"/>
       <c r="AJ14" s="7"/>
       <c r="AK14" s="7"/>
-      <c r="AL14" s="3"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>23</v>
+      <c r="AL14" s="7"/>
+      <c r="AM14" s="7"/>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>1.4</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C15" s="10">
         <v>45840</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="10">
-        <v>45840</v>
+      <c r="D15" s="6">
+        <v>1</v>
+      </c>
+      <c r="E15" s="11">
+        <f t="shared" si="1"/>
+        <v>45841</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="17"/>
+      <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
@@ -1511,25 +1570,29 @@
       <c r="AI15" s="7"/>
       <c r="AJ15" s="7"/>
       <c r="AK15" s="7"/>
-      <c r="AL15" s="3"/>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="6"/>
+      <c r="AL15" s="7"/>
+      <c r="AM15" s="7"/>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="10">
+        <v>45841</v>
+      </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="E16" s="10">
+        <v>45841</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="L16" s="17"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
@@ -1555,24 +1618,19 @@
       <c r="AI16" s="7"/>
       <c r="AJ16" s="7"/>
       <c r="AK16" s="7"/>
-      <c r="AL16" s="3"/>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
-        <v>2.1</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="10">
-        <v>45840</v>
-      </c>
-      <c r="D17" s="6">
-        <v>2</v>
-      </c>
-      <c r="E17" s="11">
+      <c r="AL16" s="7"/>
+      <c r="AM16" s="7"/>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>45842</v>
+        <v/>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -1605,24 +1663,25 @@
       <c r="AI17" s="7"/>
       <c r="AJ17" s="7"/>
       <c r="AK17" s="7"/>
-      <c r="AL17" s="3"/>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL17" s="7"/>
+      <c r="AM17" s="7"/>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C18" s="10">
-        <v>45842</v>
+        <v>45841</v>
       </c>
       <c r="D18" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E18" s="11">
         <f t="shared" si="1"/>
-        <v>45848</v>
+        <v>45843</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
@@ -1655,21 +1714,25 @@
       <c r="AI18" s="7"/>
       <c r="AJ18" s="7"/>
       <c r="AK18" s="7"/>
-      <c r="AL18" s="3"/>
-    </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL18" s="7"/>
+      <c r="AM18" s="7"/>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C19" s="10">
-        <v>45848</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="10">
-        <v>45848</v>
+        <v>45843</v>
+      </c>
+      <c r="D19" s="6">
+        <v>2</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" si="1"/>
+        <v>45845</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -1683,7 +1746,7 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
-      <c r="S19" s="17"/>
+      <c r="S19" s="7"/>
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
       <c r="V19" s="7"/>
@@ -1702,24 +1765,25 @@
       <c r="AI19" s="7"/>
       <c r="AJ19" s="7"/>
       <c r="AK19" s="7"/>
-      <c r="AL19" s="3"/>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL19" s="7"/>
+      <c r="AM19" s="7"/>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>2.2999999999999998</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C20" s="10">
-        <v>45848</v>
+        <v>45845</v>
       </c>
       <c r="D20" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="11">
         <f t="shared" si="1"/>
-        <v>45850</v>
+        <v>45846</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -1752,21 +1816,25 @@
       <c r="AI20" s="7"/>
       <c r="AJ20" s="7"/>
       <c r="AK20" s="7"/>
-      <c r="AL20" s="3"/>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL20" s="7"/>
+      <c r="AM20" s="7"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C21" s="10">
-        <v>45850</v>
-      </c>
-      <c r="D21" s="6"/>
+        <v>45846</v>
+      </c>
+      <c r="D21" s="6">
+        <v>3</v>
+      </c>
       <c r="E21" s="11">
-        <v>45850</v>
+        <f t="shared" si="1"/>
+        <v>45849</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -1780,9 +1848,9 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
+      <c r="S21" s="19"/>
       <c r="T21" s="7"/>
-      <c r="U21" s="17"/>
+      <c r="U21" s="7"/>
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
@@ -1799,18 +1867,25 @@
       <c r="AI21" s="7"/>
       <c r="AJ21" s="7"/>
       <c r="AK21" s="7"/>
-      <c r="AL21" s="3"/>
-    </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="11" t="str">
+      <c r="AL21" s="7"/>
+      <c r="AM21" s="7"/>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="10">
+        <v>45849</v>
+      </c>
+      <c r="D22" s="6">
+        <v>5</v>
+      </c>
+      <c r="E22" s="11">
         <f t="shared" si="1"/>
-        <v/>
+        <v>45854</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -1824,7 +1899,7 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
+      <c r="S22" s="19"/>
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
       <c r="V22" s="7"/>
@@ -1843,23 +1918,25 @@
       <c r="AI22" s="7"/>
       <c r="AJ22" s="7"/>
       <c r="AK22" s="7"/>
-      <c r="AL22" s="3"/>
-    </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
-        <v>3.1</v>
+      <c r="AL22" s="7"/>
+      <c r="AM22" s="7"/>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C23" s="10">
-        <v>45850</v>
+        <v>45854</v>
       </c>
       <c r="D23" s="6">
         <v>2</v>
       </c>
       <c r="E23" s="11">
-        <v>45851</v>
+        <f t="shared" si="1"/>
+        <v>45856</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -1873,7 +1950,7 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
+      <c r="S23" s="19"/>
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
       <c r="V23" s="7"/>
@@ -1892,21 +1969,22 @@
       <c r="AI23" s="7"/>
       <c r="AJ23" s="7"/>
       <c r="AK23" s="7"/>
-      <c r="AL23" s="3"/>
-    </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL23" s="7"/>
+      <c r="AM23" s="7"/>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C24" s="10">
-        <v>45851</v>
+        <v>45856</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="10">
-        <v>45851</v>
+        <v>45856</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -1923,12 +2001,12 @@
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
-      <c r="V24" s="17"/>
+      <c r="V24" s="7"/>
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
       <c r="Y24" s="7"/>
       <c r="Z24" s="7"/>
-      <c r="AA24" s="7"/>
+      <c r="AA24" s="17"/>
       <c r="AB24" s="7"/>
       <c r="AC24" s="7"/>
       <c r="AD24" s="7"/>
@@ -1939,24 +2017,25 @@
       <c r="AI24" s="7"/>
       <c r="AJ24" s="7"/>
       <c r="AK24" s="7"/>
-      <c r="AL24" s="3"/>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL24" s="7"/>
+      <c r="AM24" s="7"/>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
-        <v>3.2</v>
+        <v>2.7</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C25" s="10">
-        <v>45851</v>
+        <v>45856</v>
       </c>
       <c r="D25" s="6">
         <v>1</v>
       </c>
       <c r="E25" s="11">
         <f t="shared" si="1"/>
-        <v>45852</v>
+        <v>45857</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
@@ -1989,24 +2068,22 @@
       <c r="AI25" s="7"/>
       <c r="AJ25" s="7"/>
       <c r="AK25" s="7"/>
-      <c r="AL25" s="3"/>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
-        <v>3.3</v>
+      <c r="AL25" s="7"/>
+      <c r="AM25" s="7"/>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="11">
-        <v>45852</v>
-      </c>
-      <c r="D26" s="6">
-        <v>1</v>
-      </c>
-      <c r="E26" s="11">
-        <f t="shared" si="1"/>
-        <v>45853</v>
+        <v>31</v>
+      </c>
+      <c r="C26" s="10">
+        <v>45857</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="10">
+        <v>45857</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
@@ -2029,7 +2106,7 @@
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
       <c r="AA26" s="7"/>
-      <c r="AB26" s="7"/>
+      <c r="AB26" s="17"/>
       <c r="AC26" s="7"/>
       <c r="AD26" s="7"/>
       <c r="AE26" s="7"/>
@@ -2039,24 +2116,19 @@
       <c r="AI26" s="7"/>
       <c r="AJ26" s="7"/>
       <c r="AK26" s="7"/>
-      <c r="AL26" s="3"/>
-    </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
-        <v>3.4</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="10">
-        <v>45853</v>
-      </c>
-      <c r="D27" s="6">
-        <v>1</v>
-      </c>
-      <c r="E27" s="11">
+      <c r="AL26" s="7"/>
+      <c r="AM26" s="7"/>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="B27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>45854</v>
+        <v/>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
@@ -2089,21 +2161,24 @@
       <c r="AI27" s="7"/>
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
-      <c r="AL27" s="3"/>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>32</v>
+      <c r="AL27" s="7"/>
+      <c r="AM27" s="7"/>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>3.1</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C28" s="10">
-        <v>45854</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="10">
-        <v>45854</v>
+        <v>45857</v>
+      </c>
+      <c r="D28" s="6">
+        <v>3</v>
+      </c>
+      <c r="E28" s="11">
+        <v>45859</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -2123,7 +2198,7 @@
       <c r="V28" s="7"/>
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
-      <c r="Y28" s="17"/>
+      <c r="Y28" s="7"/>
       <c r="Z28" s="7"/>
       <c r="AA28" s="7"/>
       <c r="AB28" s="7"/>
@@ -2136,24 +2211,24 @@
       <c r="AI28" s="7"/>
       <c r="AJ28" s="7"/>
       <c r="AK28" s="7"/>
-      <c r="AL28" s="3"/>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
-        <v>3.5</v>
+      <c r="AL28" s="7"/>
+      <c r="AM28" s="7"/>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C29" s="10">
-        <v>45854</v>
+        <v>45859</v>
       </c>
       <c r="D29" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" s="11">
-        <f t="shared" si="1"/>
-        <v>45855</v>
+        <v>45861</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -2170,7 +2245,7 @@
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
-      <c r="V29" s="7"/>
+      <c r="V29" s="19"/>
       <c r="W29" s="7"/>
       <c r="X29" s="7"/>
       <c r="Y29" s="7"/>
@@ -2186,24 +2261,22 @@
       <c r="AI29" s="7"/>
       <c r="AJ29" s="7"/>
       <c r="AK29" s="7"/>
-      <c r="AL29" s="3"/>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
-        <v>3.6</v>
+      <c r="AL29" s="7"/>
+      <c r="AM29" s="7"/>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="10">
-        <v>45855</v>
-      </c>
-      <c r="D30" s="6">
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C30" s="11">
+        <v>45861</v>
+      </c>
+      <c r="D30" s="6"/>
       <c r="E30" s="11">
-        <f>IF(C30&gt;=0.01,C30+D30,"")</f>
-        <v>45856</v>
+        <v>45861</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
@@ -2230,26 +2303,31 @@
       <c r="AC30" s="7"/>
       <c r="AD30" s="7"/>
       <c r="AE30" s="7"/>
-      <c r="AF30" s="7"/>
+      <c r="AF30" s="17"/>
       <c r="AG30" s="7"/>
       <c r="AH30" s="7"/>
       <c r="AI30" s="7"/>
       <c r="AJ30" s="7"/>
       <c r="AK30" s="7"/>
-      <c r="AL30" s="3"/>
-    </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>38</v>
+      <c r="AL30" s="7"/>
+      <c r="AM30" s="7"/>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>3.2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C31" s="10">
-        <v>45856</v>
-      </c>
-      <c r="E31" s="10">
-        <v>45856</v>
+        <v>45861</v>
+      </c>
+      <c r="D31" s="6">
+        <v>2</v>
+      </c>
+      <c r="E31" s="11">
+        <f t="shared" si="1"/>
+        <v>45863</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
@@ -2270,7 +2348,8 @@
       <c r="W31" s="7"/>
       <c r="X31" s="7"/>
       <c r="Y31" s="7"/>
-      <c r="AA31" s="17"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7"/>
       <c r="AB31" s="7"/>
       <c r="AC31" s="7"/>
       <c r="AD31" s="7"/>
@@ -2281,62 +2360,393 @@
       <c r="AI31" s="7"/>
       <c r="AJ31" s="7"/>
       <c r="AK31" s="7"/>
-      <c r="AL31" s="3"/>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D32" s="6"/>
+      <c r="AL31" s="7"/>
+      <c r="AM31" s="7"/>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="11">
+        <v>45863</v>
+      </c>
+      <c r="D32" s="6">
+        <v>1</v>
+      </c>
+      <c r="E32" s="11">
+        <f t="shared" si="1"/>
+        <v>45864</v>
+      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
       <c r="Z32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="AA32" s="7"/>
+      <c r="AB32" s="7"/>
+      <c r="AC32" s="7"/>
+      <c r="AD32" s="7"/>
+      <c r="AE32" s="7"/>
+      <c r="AF32" s="7"/>
+      <c r="AG32" s="7"/>
+      <c r="AH32" s="7"/>
+      <c r="AI32" s="7"/>
+      <c r="AJ32" s="7"/>
+      <c r="AK32" s="7"/>
+      <c r="AL32" s="7"/>
+      <c r="AM32" s="7"/>
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>3.3</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="10">
+        <v>45864</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1</v>
+      </c>
+      <c r="E33" s="11">
+        <f t="shared" si="1"/>
+        <v>45865</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7"/>
+      <c r="AC33" s="7"/>
+      <c r="AD33" s="7"/>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
+      <c r="AJ33" s="7"/>
+      <c r="AK33" s="7"/>
+      <c r="AL33" s="7"/>
+      <c r="AM33" s="7"/>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="10">
+        <v>45864</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10">
+        <v>45865</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="7"/>
+      <c r="AE34" s="7"/>
+      <c r="AF34" s="7"/>
+      <c r="AG34" s="7"/>
+      <c r="AH34" s="7"/>
+      <c r="AI34" s="7"/>
+      <c r="AJ34" s="7"/>
+      <c r="AK34" s="7"/>
+      <c r="AL34" s="7"/>
+      <c r="AM34" s="7"/>
+    </row>
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="10">
+        <v>45865</v>
+      </c>
+      <c r="D35" s="6">
+        <v>1</v>
+      </c>
+      <c r="E35" s="11">
+        <f t="shared" si="1"/>
+        <v>45866</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7"/>
+      <c r="AC35" s="7"/>
+      <c r="AD35" s="7"/>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="7"/>
+      <c r="AJ35" s="7"/>
+      <c r="AK35" s="7"/>
+      <c r="AL35" s="7"/>
+      <c r="AM35" s="7"/>
+    </row>
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="10">
+        <v>45866</v>
+      </c>
+      <c r="D36" s="6">
+        <v>1</v>
+      </c>
+      <c r="E36" s="11">
+        <f>IF(C36&gt;=0.01,C36+D36,"")</f>
+        <v>45867</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="7"/>
+      <c r="AB36" s="7"/>
+      <c r="AC36" s="7"/>
+      <c r="AD36" s="7"/>
+      <c r="AE36" s="7"/>
+      <c r="AF36" s="7"/>
+      <c r="AG36" s="7"/>
+      <c r="AH36" s="7"/>
+      <c r="AI36" s="7"/>
+      <c r="AJ36" s="7"/>
+      <c r="AK36" s="20"/>
+      <c r="AL36" s="7"/>
+      <c r="AM36" s="7"/>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="10">
+        <v>45867</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1</v>
+      </c>
+      <c r="E37" s="11">
+        <f>IF(C37&gt;=0.01,C37+D37,"")</f>
+        <v>45868</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="7"/>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="19"/>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7"/>
+      <c r="AC37" s="7"/>
+      <c r="AD37" s="7"/>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
+      <c r="AJ37" s="7"/>
+      <c r="AK37" s="7"/>
+      <c r="AL37" s="7"/>
+      <c r="AM37" s="7"/>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="10">
+        <v>45868</v>
+      </c>
+      <c r="E38" s="10">
+        <v>45868</v>
+      </c>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="7"/>
+      <c r="AG38" s="7"/>
+      <c r="AH38" s="7"/>
+      <c r="AI38" s="7"/>
+      <c r="AJ38" s="7"/>
+      <c r="AK38" s="7"/>
+      <c r="AL38" s="7"/>
+      <c r="AM38" s="17"/>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="Z39" s="7"/>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A41" s="16"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" s="16"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D48" s="6"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
@@ -2377,43 +2787,136 @@
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="6"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="6"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="6"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="6"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="6"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="6"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <conditionalFormatting sqref="G8:AK8">
-    <cfRule type="expression" dxfId="3" priority="7">
+  <conditionalFormatting sqref="Z39 AK36">
+    <cfRule type="expression" dxfId="11" priority="37">
+      <formula>AND(NOT(ISBLANK($C35)),Z$8&gt;=$C35,Z$8&lt;=$E35)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="38">
+      <formula>ISBLANK(V$11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:AM8">
+    <cfRule type="expression" dxfId="10" priority="22">
       <formula>WEEKDAY(G$8)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:AK14 G15:J15 L15:AK15 G16:AK18 G19:R19 T19:AK19 G20:AK20 Z28:AK28 G22:AK23 G21:T21 V21:AK21 G25:AK27 G24:U24 W24:AK24 G28:X28 G29:AK29 Z30:AA30">
-    <cfRule type="expression" dxfId="2" priority="12">
+  <conditionalFormatting sqref="G11:AK15 M16:AK16 G17:AK23 G25:AK25 G27:AK29 Z36:AA37 AG30:AK30 G16:K16 AB24:AK24 G24:Z24 AC26:AK26 G26:AA26 G30:AE30 G31:AK35">
+    <cfRule type="expression" dxfId="9" priority="27">
       <formula>AND(NOT(ISBLANK($C11)),G$8&gt;=$C11,G$8&lt;=$E11)</formula>
     </cfRule>
-    <cfRule type="expression" priority="13">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:AK15 M16:AK16 G25:AK25 G27:AK29 G17:AK23 AG30:AK30 G36:AI36 G16:K16 AB24:AK24 G24:Z24 AC26:AK26 G26:AA26 G30:AE30 G31:AK35 G37:AK37">
+    <cfRule type="expression" priority="28">
       <formula>ISBLANK(C$11)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G31:Y31 Z32 AB31:AK31">
-    <cfRule type="expression" dxfId="1" priority="22">
-      <formula>AND(NOT(ISBLANK($C30)),G$8&gt;=$C30,G$8&lt;=$E30)</formula>
+  <conditionalFormatting sqref="G36:AI36 G37:AH37">
+    <cfRule type="expression" dxfId="8" priority="39">
+      <formula>AND(NOT(ISBLANK(#REF!)),G$8&gt;=#REF!,G$8&lt;=#REF!)</formula>
     </cfRule>
-    <cfRule type="expression" priority="23">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA38">
+    <cfRule type="expression" priority="12">
+      <formula>ISBLANK(W$11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA38">
+    <cfRule type="expression" dxfId="7" priority="13">
+      <formula>AND(NOT(ISBLANK(#REF!)),AA$8&gt;=#REF!,AA$8&lt;=#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ38">
+    <cfRule type="expression" priority="10">
+      <formula>ISBLANK(AF$11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ38">
+    <cfRule type="expression" dxfId="6" priority="11">
+      <formula>AND(NOT(ISBLANK(#REF!)),AJ$8&gt;=#REF!,AJ$8&lt;=#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB38:AI38 G38:Y38">
+    <cfRule type="expression" dxfId="5" priority="40">
+      <formula>AND(NOT(ISBLANK($C36)),G$8&gt;=$C36,G$8&lt;=$E36)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="41">
       <formula>ISBLANK(C$11)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G30:AK30">
-    <cfRule type="expression" dxfId="0" priority="24">
-      <formula>AND(NOT(ISBLANK(#REF!)),G$8&gt;=#REF!,G$8&lt;=#REF!)</formula>
+  <conditionalFormatting sqref="AL11:AL38">
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>AND(NOT(ISBLANK($C11)),AL$8&gt;=$C11,AL$8&lt;=$E11)</formula>
     </cfRule>
-    <cfRule type="expression" priority="25">
-      <formula>ISBLANK(C$11)</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL11:AL38">
+    <cfRule type="expression" priority="9">
+      <formula>ISBLANK(AH$11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM11:AM37">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>AND(NOT(ISBLANK($C11)),AM$8&gt;=$C11,AM$8&lt;=$E11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM11:AM37">
+    <cfRule type="expression" priority="7">
+      <formula>ISBLANK(AI$11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK38">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>AND(NOT(ISBLANK($C38)),AK$8&gt;=$C38,AK$8&lt;=$E38)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK38">
+    <cfRule type="expression" priority="5">
+      <formula>ISBLANK(AG$11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ36">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND(NOT(ISBLANK($C36)),AJ$8&gt;=$C36,AJ$8&lt;=$E36)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ36">
+    <cfRule type="expression" priority="3">
+      <formula>ISBLANK(AF$11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI37:AK37">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(NOT(ISBLANK($C37)),AI$8&gt;=$C37,AI$8&lt;=$E37)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.53740157499999996" bottom="0.53740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="67" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="67" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>